<commit_message>
receita e despesa dividida
</commit_message>
<xml_diff>
--- a/GV_2025-01.xlsx
+++ b/GV_2025-01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,6 +555,46 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Despesa</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SERVIÇOS</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>26/01/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Receita</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ALUGUEL</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>26/01/2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
dashboard sem a % dos socios
</commit_message>
<xml_diff>
--- a/GV_2025-01.xlsx
+++ b/GV_2025-01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,26 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Despesa</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SERVIÇOS</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>50</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>26/01/2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
saldo proximo mes negativo corretamente
</commit_message>
<xml_diff>
--- a/GV_2025-01.xlsx
+++ b/GV_2025-01.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,165 +458,31 @@
           <t>Data</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Saldo Inicial</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Despesa</t>
+          <t>Saldo Inicial</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ESCRITÓRIO</t>
+          <t>Inicial</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>25/01/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Despesa</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ESCRITÓRIO</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>600</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>25/01/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Receita</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ALUGUEL</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>900</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>25/01/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Receita</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ALUGUEL</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>25/01/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Receita</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>APLICAÇÕES FINANCEIRAS</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>25/01/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Despesa</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SERVIÇOS</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>50</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>26/01/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Receita</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ALUGUEL</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>26/01/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Despesa</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SERVIÇOS</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>50</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>26/01/2025</t>
-        </is>
+        <v>-3500</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45658</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-3500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
faltando transferir receita botao n ta aparecendo
</commit_message>
<xml_diff>
--- a/GV_2025-01.xlsx
+++ b/GV_2025-01.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,122 +463,26 @@
           <t>Saldo Inicial</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Inquilino</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Despesa</t>
+          <t>Saldo Inicial</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>EQUIPAMENTOS</t>
+          <t>Inicial</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>250</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>26/01/2025</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45658</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Receita</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>APLICAÇÕES FINANCEIRAS</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>500</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>26/01/2025</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Joao</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Despesa</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SERVIÇOS</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>100</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>29/01/2025</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Despesa</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SERVIÇOS</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>100</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>29/01/2025</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>